<commit_message>
Se actualizan archivos, se incluyen funciones para generar archivos
</commit_message>
<xml_diff>
--- a/Planillas/p1_sample.xlsx
+++ b/Planillas/p1_sample.xlsx
@@ -5,7 +5,7 @@
     <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId4"/>
+    <sheet name="DEPOR" sheetId="1" r:id="rId4"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId5"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId6"/>
   </sheets>
@@ -278,7 +278,7 @@
     <font>
       <b val="1"/>
       <sz val="8"/>
-      <color indexed="9"/>
+      <color indexed="10"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -302,7 +302,7 @@
       <b val="1"/>
       <i val="1"/>
       <sz val="12"/>
-      <color indexed="9"/>
+      <color indexed="10"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -315,7 +315,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="10"/>
+        <fgColor indexed="9"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -326,7 +326,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -353,6 +353,93 @@
       <left style="thin">
         <color indexed="12"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="12"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="12"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="12"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="12"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
       <right style="thin">
         <color indexed="12"/>
       </right>
@@ -370,14 +457,14 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -392,37 +479,34 @@
     <xf numFmtId="49" fontId="5" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="6" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="6" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="6" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="6" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="7" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -431,16 +515,43 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="8" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -463,8 +574,8 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ff1f497d"/>
-      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ff92d050"/>
       <rgbColor rgb="ffaaaaaa"/>
     </indexedColors>
@@ -617,9 +728,9 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -699,7 +810,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -727,10 +838,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -986,9 +1097,9 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
             <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
+              <a:alpha val="35000"/>
             </a:srgbClr>
           </a:outerShdw>
         </a:effectLst>
@@ -1276,7 +1387,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1304,10 +1415,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1558,7 +1669,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:Z4"/>
+  <dimension ref="A1:Z10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1732,7 +1843,7 @@
       <c r="Y2" t="s" s="15">
         <v>42</v>
       </c>
-      <c r="Z2" s="16"/>
+      <c r="Z2" s="12"/>
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" t="s" s="8">
@@ -1783,7 +1894,7 @@
       <c r="P3" t="s" s="8">
         <v>51</v>
       </c>
-      <c r="Q3" t="s" s="17">
+      <c r="Q3" t="s" s="16">
         <v>52</v>
       </c>
       <c r="R3" t="s" s="10">
@@ -1795,17 +1906,17 @@
       <c r="T3" t="s" s="10">
         <v>55</v>
       </c>
-      <c r="U3" s="18">
+      <c r="U3" s="17">
         <v>44260</v>
       </c>
-      <c r="V3" s="18">
+      <c r="V3" s="17">
         <v>44261</v>
       </c>
       <c r="W3" t="s" s="13">
         <v>56</v>
       </c>
-      <c r="X3" s="19"/>
-      <c r="Y3" s="20">
+      <c r="X3" s="18"/>
+      <c r="Y3" s="19">
         <v>10568154</v>
       </c>
       <c r="Z3" t="s" s="15">
@@ -1861,7 +1972,7 @@
       <c r="P4" t="s" s="8">
         <v>66</v>
       </c>
-      <c r="Q4" t="s" s="17">
+      <c r="Q4" t="s" s="16">
         <v>52</v>
       </c>
       <c r="R4" t="s" s="10">
@@ -1874,21 +1985,189 @@
         <v>55</v>
       </c>
       <c r="U4" s="12"/>
-      <c r="V4" s="18">
+      <c r="V4" s="17">
         <v>44247</v>
       </c>
       <c r="W4" t="s" s="13">
         <v>68</v>
       </c>
-      <c r="X4" s="21">
+      <c r="X4" s="20">
         <v>974048940</v>
       </c>
-      <c r="Y4" s="20">
+      <c r="Y4" s="19">
         <v>10496521</v>
       </c>
       <c r="Z4" t="s" s="15">
         <v>57</v>
       </c>
+    </row>
+    <row r="5" ht="13.55" customHeight="1">
+      <c r="A5" s="21"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="22"/>
+      <c r="M5" s="22"/>
+      <c r="N5" s="22"/>
+      <c r="O5" s="22"/>
+      <c r="P5" s="22"/>
+      <c r="Q5" s="22"/>
+      <c r="R5" s="22"/>
+      <c r="S5" s="22"/>
+      <c r="T5" s="22"/>
+      <c r="U5" s="22"/>
+      <c r="V5" s="22"/>
+      <c r="W5" s="22"/>
+      <c r="X5" s="22"/>
+      <c r="Y5" s="22"/>
+      <c r="Z5" s="23"/>
+    </row>
+    <row r="6" ht="13.55" customHeight="1">
+      <c r="A6" s="24"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+      <c r="H6" s="25"/>
+      <c r="I6" s="25"/>
+      <c r="J6" s="25"/>
+      <c r="K6" s="25"/>
+      <c r="L6" s="25"/>
+      <c r="M6" s="25"/>
+      <c r="N6" s="25"/>
+      <c r="O6" s="25"/>
+      <c r="P6" s="25"/>
+      <c r="Q6" s="25"/>
+      <c r="R6" s="25"/>
+      <c r="S6" s="25"/>
+      <c r="T6" s="25"/>
+      <c r="U6" s="25"/>
+      <c r="V6" s="25"/>
+      <c r="W6" s="25"/>
+      <c r="X6" s="25"/>
+      <c r="Y6" s="25"/>
+      <c r="Z6" s="26"/>
+    </row>
+    <row r="7" ht="13.55" customHeight="1">
+      <c r="A7" s="24"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
+      <c r="I7" s="25"/>
+      <c r="J7" s="25"/>
+      <c r="K7" s="25"/>
+      <c r="L7" s="25"/>
+      <c r="M7" s="25"/>
+      <c r="N7" s="25"/>
+      <c r="O7" s="25"/>
+      <c r="P7" s="25"/>
+      <c r="Q7" s="25"/>
+      <c r="R7" s="25"/>
+      <c r="S7" s="25"/>
+      <c r="T7" s="25"/>
+      <c r="U7" s="25"/>
+      <c r="V7" s="25"/>
+      <c r="W7" s="25"/>
+      <c r="X7" s="25"/>
+      <c r="Y7" s="25"/>
+      <c r="Z7" s="26"/>
+    </row>
+    <row r="8" ht="13.55" customHeight="1">
+      <c r="A8" s="24"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="25"/>
+      <c r="K8" s="25"/>
+      <c r="L8" s="25"/>
+      <c r="M8" s="25"/>
+      <c r="N8" s="25"/>
+      <c r="O8" s="25"/>
+      <c r="P8" s="25"/>
+      <c r="Q8" s="25"/>
+      <c r="R8" s="25"/>
+      <c r="S8" s="25"/>
+      <c r="T8" s="25"/>
+      <c r="U8" s="25"/>
+      <c r="V8" s="25"/>
+      <c r="W8" s="25"/>
+      <c r="X8" s="25"/>
+      <c r="Y8" s="25"/>
+      <c r="Z8" s="26"/>
+    </row>
+    <row r="9" ht="13.55" customHeight="1">
+      <c r="A9" s="24"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="25"/>
+      <c r="L9" s="25"/>
+      <c r="M9" s="25"/>
+      <c r="N9" s="25"/>
+      <c r="O9" s="25"/>
+      <c r="P9" s="25"/>
+      <c r="Q9" s="25"/>
+      <c r="R9" s="25"/>
+      <c r="S9" s="25"/>
+      <c r="T9" s="25"/>
+      <c r="U9" s="25"/>
+      <c r="V9" s="25"/>
+      <c r="W9" s="25"/>
+      <c r="X9" s="25"/>
+      <c r="Y9" s="25"/>
+      <c r="Z9" s="26"/>
+    </row>
+    <row r="10" ht="13.55" customHeight="1">
+      <c r="A10" s="27"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="28"/>
+      <c r="L10" s="28"/>
+      <c r="M10" s="28"/>
+      <c r="N10" s="28"/>
+      <c r="O10" s="28"/>
+      <c r="P10" s="28"/>
+      <c r="Q10" s="28"/>
+      <c r="R10" s="28"/>
+      <c r="S10" s="28"/>
+      <c r="T10" s="28"/>
+      <c r="U10" s="28"/>
+      <c r="V10" s="28"/>
+      <c r="W10" s="28"/>
+      <c r="X10" s="28"/>
+      <c r="Y10" s="28"/>
+      <c r="Z10" s="29"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1912,79 +2191,79 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="5" width="10.8516" style="22" customWidth="1"/>
-    <col min="6" max="16384" width="10.8516" style="22" customWidth="1"/>
+    <col min="1" max="5" width="10.8516" style="30" customWidth="1"/>
+    <col min="6" max="16384" width="10.8516" style="30" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.55" customHeight="1">
-      <c r="A1" s="23"/>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
+      <c r="A1" s="31"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
     </row>
     <row r="2" ht="13.55" customHeight="1">
-      <c r="A2" s="23"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="A2" s="31"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
     </row>
     <row r="3" ht="13.55" customHeight="1">
-      <c r="A3" s="23"/>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
+      <c r="A3" s="31"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
     </row>
     <row r="4" ht="13.55" customHeight="1">
-      <c r="A4" s="23"/>
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
+      <c r="A4" s="31"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
     </row>
     <row r="5" ht="13.55" customHeight="1">
-      <c r="A5" s="23"/>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
+      <c r="A5" s="31"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
     </row>
     <row r="6" ht="13.55" customHeight="1">
-      <c r="A6" s="23"/>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
+      <c r="A6" s="31"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
     </row>
     <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" s="23"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
+      <c r="A7" s="31"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
     </row>
     <row r="8" ht="13.55" customHeight="1">
-      <c r="A8" s="23"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
+      <c r="A8" s="31"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
     </row>
     <row r="9" ht="13.55" customHeight="1">
-      <c r="A9" s="23"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
+      <c r="A9" s="31"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
     </row>
     <row r="10" ht="13.55" customHeight="1">
-      <c r="A10" s="23"/>
-      <c r="B10" s="23"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
+      <c r="A10" s="31"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2003,79 +2282,79 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="5" width="10.8516" style="24" customWidth="1"/>
-    <col min="6" max="16384" width="10.8516" style="24" customWidth="1"/>
+    <col min="1" max="5" width="10.8516" style="32" customWidth="1"/>
+    <col min="6" max="16384" width="10.8516" style="32" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.55" customHeight="1">
-      <c r="A1" s="23"/>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
+      <c r="A1" s="31"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
     </row>
     <row r="2" ht="13.55" customHeight="1">
-      <c r="A2" s="23"/>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="A2" s="31"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
     </row>
     <row r="3" ht="13.55" customHeight="1">
-      <c r="A3" s="23"/>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
+      <c r="A3" s="31"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
     </row>
     <row r="4" ht="13.55" customHeight="1">
-      <c r="A4" s="23"/>
-      <c r="B4" s="23"/>
-      <c r="C4" s="23"/>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23"/>
+      <c r="A4" s="31"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
     </row>
     <row r="5" ht="13.55" customHeight="1">
-      <c r="A5" s="23"/>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23"/>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
+      <c r="A5" s="31"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
     </row>
     <row r="6" ht="13.55" customHeight="1">
-      <c r="A6" s="23"/>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
+      <c r="A6" s="31"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
     </row>
     <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" s="23"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
+      <c r="A7" s="31"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
     </row>
     <row r="8" ht="13.55" customHeight="1">
-      <c r="A8" s="23"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
+      <c r="A8" s="31"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
     </row>
     <row r="9" ht="13.55" customHeight="1">
-      <c r="A9" s="23"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
+      <c r="A9" s="31"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
     </row>
     <row r="10" ht="13.55" customHeight="1">
-      <c r="A10" s="23"/>
-      <c r="B10" s="23"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
+      <c r="A10" s="31"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>